<commit_message>
Se tiene primer entregable considerando los drops y el DELTA
</commit_message>
<xml_diff>
--- a/prueba.xlsx
+++ b/prueba.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="movil_prioridad_zona" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,25 +436,40 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>codunico</t>
+          <t>Departamento</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>detalle</t>
+          <t>Nombre Sitio</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Tipo de Sitio HISPAM</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>zona</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>ID_UNICO</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>ESPECIALIDAD</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>PROBLEMA</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>ACCIONES</t>
         </is>
@@ -463,25 +478,40 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>LI01649</t>
+          <t>LIMA</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 29- Drops 4g: 89- Sector: 1</t>
+          <t>CENTRO CIVICO</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Zona 2</t>
+          <t>B_2</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>RADIO-RADIO</t>
+          <t>Zona 1</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
+        <is>
+          <t>LI00353</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>RADIO-RADIO</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 28.86399999999999- Drops 4g: 468- Sector: 1</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
         <is>
           <t>EN SITIO REVISAR Y CORRECCION DE PROBLEMA REPORTADO POR CALIDAD MOVIL</t>
         </is>
@@ -490,25 +520,40 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>LI00357</t>
+          <t>LIMA</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 26- Drops 4g: 54- Sector: 2</t>
+          <t>FACULTAD</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Zona 2</t>
+          <t>B_2</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>RADIO-RADIO</t>
+          <t>Zona 1</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
+        <is>
+          <t>LI00810</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>RADIO-RADIO</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 3.632000000000005- Drops 4g: 307- Sector: 3</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
         <is>
           <t>EN SITIO REVISAR Y CORRECCION DE PROBLEMA REPORTADO POR CALIDAD MOVIL</t>
         </is>
@@ -517,25 +562,40 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>LI06070</t>
+          <t>CALLAO</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 24- Drops 4g: 1230- Sector: 3</t>
+          <t>ALAMEDA_CENTRAL</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Zona 2</t>
+          <t>B_2</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>RADIO-RADIO</t>
+          <t>Zona 1</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
+        <is>
+          <t>LI04724</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>RADIO-RADIO</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 3.6539999999999964- Drops 4g: 74- Sector: 2</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
         <is>
           <t>EN SITIO REVISAR Y CORRECCION DE PROBLEMA REPORTADO POR CALIDAD MOVIL</t>
         </is>
@@ -544,25 +604,40 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>LI04585</t>
+          <t>CALLAO</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 19- Drops 4g: 6- Sector: 3</t>
+          <t>BASE NAVAL DEL CALLAO</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Zona 2</t>
+          <t>B_2</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>RADIO-RADIO</t>
+          <t>Zona 1</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
+        <is>
+          <t>LI00614</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>RADIO-RADIO</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 10.840000000000003- Drops 4g: 71- Sector: 2</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
         <is>
           <t>EN SITIO REVISAR Y CORRECCION DE PROBLEMA REPORTADO POR CALIDAD MOVIL</t>
         </is>
@@ -571,25 +646,40 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>LI00398</t>
+          <t>CALLAO</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 18- Drops 4g: 82- Sector: 3</t>
+          <t>PARQUE_INDUSTRIAL_VENTANILLA</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Zona 2</t>
+          <t>B_2</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>RADIO-RADIO</t>
+          <t>Zona 1</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
+        <is>
+          <t>LI05850</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>RADIO-RADIO</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 19.897999999999996- Drops 4g: 68- Sector: 2</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
         <is>
           <t>EN SITIO REVISAR Y CORRECCION DE PROBLEMA REPORTADO POR CALIDAD MOVIL</t>
         </is>
@@ -598,25 +688,40 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>LI01713</t>
+          <t>LIMA</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 17- Drops 4g: 1- Sector: 2</t>
+          <t>ABANCAY CLARO (MURALLA)</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Zona 2</t>
+          <t>B_2</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>RADIO-RADIO</t>
+          <t>Zona 1</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
+        <is>
+          <t>LI00943</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>RADIO-RADIO</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 5.212999999999994- Drops 4g: 66- Sector: 3</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
         <is>
           <t>EN SITIO REVISAR Y CORRECCION DE PROBLEMA REPORTADO POR CALIDAD MOVIL</t>
         </is>
@@ -625,25 +730,40 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>LI00413</t>
+          <t>LIMA</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 16- Drops 4g: 78- Sector: 4</t>
+          <t>AMAZONAS_PARURO</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Zona 2</t>
+          <t>B_2</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>RADIO-RADIO</t>
+          <t>Zona 1</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
+        <is>
+          <t>LI06061</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>RADIO-RADIO</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 2.034000000000006- Drops 4g: 65- Sector: 2</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
         <is>
           <t>EN SITIO REVISAR Y CORRECCION DE PROBLEMA REPORTADO POR CALIDAD MOVIL</t>
         </is>
@@ -652,25 +772,40 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>LI00552</t>
+          <t>LIMA</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 14- Drops 4g: 419- Sector: 2</t>
+          <t>INSURGENTES_LI</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Zona 2</t>
+          <t>B_1</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>RADIO-RADIO</t>
+          <t>Zona 1</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
+        <is>
+          <t>LI01626</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>RADIO-RADIO</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 2.534000000000006- Drops 4g: 61- Sector: 1*- Delta RTWP: 3.3359999999999985- Drops 4g: 17- Sector: 2</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
         <is>
           <t>EN SITIO REVISAR Y CORRECCION DE PROBLEMA REPORTADO POR CALIDAD MOVIL</t>
         </is>
@@ -679,25 +814,40 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>LI00572</t>
+          <t>LIMA</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 13- Drops 4g: 141- Sector: 1</t>
+          <t>PRECURSORES SAN MIGUEL</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Zona 2</t>
+          <t>B_2</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>RADIO-RADIO</t>
+          <t>Zona 1</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
+        <is>
+          <t>LI00828</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>RADIO-RADIO</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 22.738- Drops 4g: 59- Sector: 3</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
         <is>
           <t>EN SITIO REVISAR Y CORRECCION DE PROBLEMA REPORTADO POR CALIDAD MOVIL</t>
         </is>
@@ -706,25 +856,40 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>LI00282</t>
+          <t>CALLAO</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 12- Drops 4g: 214- Sector: 1</t>
+          <t>MI_PERU_REEM</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Zona 2</t>
+          <t>B_2</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>RADIO-RADIO</t>
+          <t>Zona 1</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
+        <is>
+          <t>LI04147</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>RADIO-RADIO</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 2.0919999999999845- Drops 4g: 41- Sector: 3</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
         <is>
           <t>EN SITIO REVISAR Y CORRECCION DE PROBLEMA REPORTADO POR CALIDAD MOVIL</t>
         </is>
@@ -733,25 +898,40 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>LI06623</t>
+          <t>LIMA</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 23- Drops 4g: 352- Sector: 2</t>
+          <t>SAN_PEDRO_CHORRILLOS</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Zona 1</t>
+          <t>B_2</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>RADIO-RADIO</t>
+          <t>Zona 2</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
+        <is>
+          <t>LI06516</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>RADIO-RADIO</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 3.5050000000000097- Drops 4g: 139- Sector: 3</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
         <is>
           <t>EN SITIO REVISAR Y CORRECCION DE PROBLEMA REPORTADO POR CALIDAD MOVIL</t>
         </is>
@@ -760,25 +940,40 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>LI00828</t>
+          <t>LIMA</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 21- Drops 4g: 23- Sector: 3</t>
+          <t>LAS VIÑAS</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Zona 1</t>
+          <t>D_1</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>RADIO-RADIO</t>
+          <t>Zona 2</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
+        <is>
+          <t>LI00039</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>RADIO-RADIO</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 2.0360000000000014- Drops 4g: 117- Sector: 2</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
         <is>
           <t>EN SITIO REVISAR Y CORRECCION DE PROBLEMA REPORTADO POR CALIDAD MOVIL</t>
         </is>
@@ -787,25 +982,40 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>LI05850</t>
+          <t>LIMA</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 20- Drops 4g: 68- Sector: 2</t>
+          <t>ANTACCASCA</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Zona 1</t>
+          <t>B_2</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>RADIO-RADIO</t>
+          <t>Zona 2</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
+        <is>
+          <t>LI06070</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>RADIO-RADIO</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 24.92900000000001- Drops 4g: 80- Sector: 3</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
         <is>
           <t>EN SITIO REVISAR Y CORRECCION DE PROBLEMA REPORTADO POR CALIDAD MOVIL</t>
         </is>
@@ -814,25 +1024,40 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>LI01187</t>
+          <t>LIMA</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 12- Drops 4g: 36- Sector: 1</t>
+          <t>LAS DUNAS MANCHAY</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Zona 1</t>
+          <t>B_2</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>RADIO-RADIO</t>
+          <t>Zona 2</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
+        <is>
+          <t>LI00517</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>RADIO-RADIO</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 5.579999999999998- Drops 4g: 69- Sector: 3</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
         <is>
           <t>EN SITIO REVISAR Y CORRECCION DE PROBLEMA REPORTADO POR CALIDAD MOVIL</t>
         </is>
@@ -841,25 +1066,40 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>LI01682</t>
+          <t>LIMA</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 9- Drops 4g: 135- Sector: 1</t>
+          <t>TORIBIO_PACHECO</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Zona 1</t>
+          <t>B_1</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>RADIO-RADIO</t>
+          <t>Zona 2</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
+        <is>
+          <t>LI05796</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>RADIO-RADIO</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 2.024000000000001- Drops 4g: 53- Sector: 2</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
         <is>
           <t>EN SITIO REVISAR Y CORRECCION DE PROBLEMA REPORTADO POR CALIDAD MOVIL</t>
         </is>
@@ -868,25 +1108,40 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>LI00969</t>
+          <t>LIMA</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 9- Drops 4g: 37- Sector: 1</t>
+          <t>LAVALLE</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Zona 1</t>
+          <t>B_2</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>RADIO-RADIO</t>
+          <t>Zona 2</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
+        <is>
+          <t>LI00718</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>RADIO-RADIO</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 3.668999999999997- Drops 4g: 50- Sector: 3</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
         <is>
           <t>EN SITIO REVISAR Y CORRECCION DE PROBLEMA REPORTADO POR CALIDAD MOVIL</t>
         </is>
@@ -895,25 +1150,40 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>LI00992</t>
+          <t>LIMA</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 9- Drops 4g: 34- Sector: 2</t>
+          <t>LOS_CABALLOS</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Zona 1</t>
+          <t>B_2</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>RADIO-RADIO</t>
+          <t>Zona 2</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
+        <is>
+          <t>LI04824</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>RADIO-RADIO</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 26.08400000000001- Drops 4g: 49- Sector: 3</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
         <is>
           <t>EN SITIO REVISAR Y CORRECCION DE PROBLEMA REPORTADO POR CALIDAD MOVIL</t>
         </is>
@@ -922,25 +1192,40 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>LI00235</t>
+          <t>LIMA</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 9- Drops 4g: 30- Sector: 3</t>
+          <t>PLAZA ARMAS NVA ESPERANZA</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Zona 1</t>
+          <t>B_2</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>RADIO-RADIO</t>
+          <t>Zona 2</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
+        <is>
+          <t>LI00633</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>RADIO-RADIO</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 3.8090000000000117- Drops 4g: 46- Sector: 1</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
         <is>
           <t>EN SITIO REVISAR Y CORRECCION DE PROBLEMA REPORTADO POR CALIDAD MOVIL</t>
         </is>
@@ -949,25 +1234,40 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>LI05986</t>
+          <t>LIMA</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 8- Drops 4g: 59- Sector: 3</t>
+          <t>LOPEZ ALBUJAR</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Zona 1</t>
+          <t>B_2</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>RADIO-RADIO</t>
+          <t>Zona 2</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
+        <is>
+          <t>LI00584</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>RADIO-RADIO</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 6.198999999999998- Drops 4g: 39- Sector: 1</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
         <is>
           <t>EN SITIO REVISAR Y CORRECCION DE PROBLEMA REPORTADO POR CALIDAD MOVIL</t>
         </is>
@@ -976,25 +1276,40 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>LI05782</t>
+          <t>LIMA</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 8- Drops 4g: 18- Sector: 1</t>
+          <t>JESUS NAZARENO</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Zona 1</t>
+          <t>B_2</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>RADIO-RADIO</t>
+          <t>Zona 2</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
+        <is>
+          <t>LI00572</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>RADIO-RADIO</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 10.361000000000004- Drops 4g: 35- Sector: 1</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
         <is>
           <t>EN SITIO REVISAR Y CORRECCION DE PROBLEMA REPORTADO POR CALIDAD MOVIL</t>
         </is>
@@ -1003,25 +1318,40 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>LI01174</t>
+          <t>LIMA</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 19- Drops 4g: 195- Sector: 3</t>
+          <t>DALIAS NORTE</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
+          <t>B_2</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
           <t>Zona 3</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>RADIO-RADIO</t>
-        </is>
-      </c>
       <c r="E22" t="inlineStr">
+        <is>
+          <t>LI00919</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>RADIO-RADIO</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 2.3430000000000035- Drops 4g: 108- Sector: 2</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
         <is>
           <t>EN SITIO REVISAR Y CORRECCION DE PROBLEMA REPORTADO POR CALIDAD MOVIL</t>
         </is>
@@ -1030,25 +1360,40 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>LI00329</t>
+          <t>LIMA</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 16- Drops 4g: 422- Sector: 1*- Delta RTWP: 13- Drops 4g: 38- Sector: 2</t>
+          <t>BELAUNDE NEW</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
+          <t>B_2</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
           <t>Zona 3</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>RADIO-RADIO</t>
-        </is>
-      </c>
       <c r="E23" t="inlineStr">
+        <is>
+          <t>LI01596</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>RADIO-RADIO</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 2.4369999999999976- Drops 4g: 78- Sector: 2*- Delta RTWP: 2.600999999999999- Drops 4g: 11- Sector: 1</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
         <is>
           <t>EN SITIO REVISAR Y CORRECCION DE PROBLEMA REPORTADO POR CALIDAD MOVIL</t>
         </is>
@@ -1057,25 +1402,40 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>LI05818</t>
+          <t>LIMA</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 9- Drops 4g: 43- Sector: 2</t>
+          <t>SAN_CRISTOBAL</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
+          <t>B_2</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
           <t>Zona 3</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>RADIO-RADIO</t>
-        </is>
-      </c>
       <c r="E24" t="inlineStr">
+        <is>
+          <t>LI05769</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>RADIO-RADIO</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 22.585000000000008- Drops 4g: 77- Sector: 1</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
         <is>
           <t>EN SITIO REVISAR Y CORRECCION DE PROBLEMA REPORTADO POR CALIDAD MOVIL</t>
         </is>
@@ -1084,25 +1444,40 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>LI00575</t>
+          <t>LIMA</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 8- Drops 4g: 61- Sector: 1</t>
+          <t>CALLES_NEW_REEM</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
+          <t>B_2</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
           <t>Zona 3</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>RADIO-RADIO</t>
-        </is>
-      </c>
       <c r="E25" t="inlineStr">
+        <is>
+          <t>LI06761</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>RADIO-RADIO</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 6.840000000000003- Drops 4g: 61- Sector: 1</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
         <is>
           <t>EN SITIO REVISAR Y CORRECCION DE PROBLEMA REPORTADO POR CALIDAD MOVIL</t>
         </is>
@@ -1111,25 +1486,40 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>LI00571</t>
+          <t>LIMA</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 8- Drops 4g: 59- Sector: 1</t>
+          <t>CC_MINA_DE_ORO</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
+          <t>B_2</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
           <t>Zona 3</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>RADIO-RADIO</t>
-        </is>
-      </c>
       <c r="E26" t="inlineStr">
+        <is>
+          <t>LI06799</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>RADIO-RADIO</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 2.378- Drops 4g: 56- Sector: 3</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
         <is>
           <t>EN SITIO REVISAR Y CORRECCION DE PROBLEMA REPORTADO POR CALIDAD MOVIL</t>
         </is>
@@ -1138,25 +1528,40 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>LI01114</t>
+          <t>LIMA</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 7- Drops 4g: 250- Sector: 2</t>
+          <t>TROMECITO</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
+          <t>B_2</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
           <t>Zona 3</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>RADIO-RADIO</t>
-        </is>
-      </c>
       <c r="E27" t="inlineStr">
+        <is>
+          <t>LI04135</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>RADIO-RADIO</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 4.0449999999999875- Drops 4g: 51- Sector: 1</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
         <is>
           <t>EN SITIO REVISAR Y CORRECCION DE PROBLEMA REPORTADO POR CALIDAD MOVIL</t>
         </is>
@@ -1165,25 +1570,40 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>LI01613</t>
+          <t>LIMA</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 7- Drops 4g: 170- Sector: 3*- Delta RTWP: 4- Drops 4g: 92- Sector: 2</t>
+          <t>ANTON SANCHEZ</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
+          <t>B_2</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
           <t>Zona 3</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>RADIO-RADIO</t>
-        </is>
-      </c>
       <c r="E28" t="inlineStr">
+        <is>
+          <t>LI00949</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>RADIO-RADIO</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 5.133999999999986- Drops 4g: 43- Sector: 3</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
         <is>
           <t>EN SITIO REVISAR Y CORRECCION DE PROBLEMA REPORTADO POR CALIDAD MOVIL</t>
         </is>
@@ -1192,25 +1612,40 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>LI01038</t>
+          <t>LIMA</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 7- Drops 4g: 116- Sector: 2</t>
+          <t>FUCSIAS_GRAU</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
+          <t>B_2</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
           <t>Zona 3</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>RADIO-RADIO</t>
-        </is>
-      </c>
       <c r="E29" t="inlineStr">
+        <is>
+          <t>LI05330</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>RADIO-RADIO</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 23.875- Drops 4g: 32- Sector: 2</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
         <is>
           <t>EN SITIO REVISAR Y CORRECCION DE PROBLEMA REPORTADO POR CALIDAD MOVIL</t>
         </is>
@@ -1219,25 +1654,40 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>LI00925</t>
+          <t>LIMA</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 7- Drops 4g: 70- Sector: 1</t>
+          <t>ARHUA</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
+          <t>B_2</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
           <t>Zona 3</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>RADIO-RADIO</t>
-        </is>
-      </c>
       <c r="E30" t="inlineStr">
+        <is>
+          <t>LI00565</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>RADIO-RADIO</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 2.4509999999999934- Drops 4g: 21- Sector: 1</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
         <is>
           <t>EN SITIO REVISAR Y CORRECCION DE PROBLEMA REPORTADO POR CALIDAD MOVIL</t>
         </is>
@@ -1246,25 +1696,40 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>LI00951</t>
+          <t>LIMA</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 7- Drops 4g: 27- Sector: 1</t>
+          <t>UCHUPATA</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
+          <t>B_2</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
           <t>Zona 3</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>RADIO-RADIO</t>
-        </is>
-      </c>
       <c r="E31" t="inlineStr">
+        <is>
+          <t>LI00569</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>RADIO-RADIO</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>*PROACTIVO CALIDAD MOVIL |*- Delta RTWP: 5.621000000000009- Drops 4g: 21- Sector: 2</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
         <is>
           <t>EN SITIO REVISAR Y CORRECCION DE PROBLEMA REPORTADO POR CALIDAD MOVIL</t>
         </is>

</xml_diff>